<commit_message>
Story 5:Edit serial fot Testing Cooler
</commit_message>
<xml_diff>
--- a/Homework_1/Cooler_Requirements_Vlad_Dmytrenko.xlsx
+++ b/Homework_1/Cooler_Requirements_Vlad_Dmytrenko.xlsx
@@ -19,70 +19,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>1. Экологичность</t>
-  </si>
-  <si>
-    <t>2. Компактность</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.Электробезопастность </t>
-  </si>
-  <si>
-    <t>4. Функциональность</t>
-  </si>
-  <si>
-    <t>5. Простота</t>
-  </si>
-  <si>
-    <t>6.Энергозберегаемость</t>
-  </si>
-  <si>
-    <t>7. Экономичность</t>
-  </si>
-  <si>
-    <t>8. Востребуемость</t>
-  </si>
-  <si>
-    <t>9. Безопастность</t>
-  </si>
-  <si>
-    <t>Корпус водного кулера производиться из экологически чистого пластмаса, который не содержит вредные элементы, а также имеет металические вставки, которые в свою очередь имеют нержавеющюю сталь.</t>
-  </si>
-  <si>
-    <t>Весь цикл работы даного прибора происходит в автоматическом режиме. Данный прибор не требует отключение от сети.</t>
-  </si>
-  <si>
-    <t>Кулер выполнен в напольном варианте и снабжен дополнительно внутренними камерами-озонаторами посуды, а также холодильной камерой.</t>
-  </si>
-  <si>
-    <t>Одной из основных функций кулера для воды являеться охлождение. Причем этот процес происходит полностью в автоматическом режиме без вмешательства пользователя. После полной заправки кулера водой, она охлождается до температуры от 5 до 13 градусов по Цельсию. Кулер для воды охлождаеться при помощи компрессора. Второй обязательной функцией кулера для воды являеться нагрев воды.После заправки, вода нагревается до температуры от 80 до 95 градусов Цельсия и, как в случае с охлаждением воды поддерживается в таком состоянии длительное время. Необязательная функция кулеров позволяет получать газировку из простой питьевой воды. Это обеспечивается за счет специального отсека, оснащенного сменной кассетой. Нельзя не упомянуть, что после того, как вы устанавливаете бутыль с водой в принимающих отсек кулера, она проходит несколько степеней очистки: механическая очистка, химическая очистка и тд.</t>
-  </si>
-  <si>
-    <t>Лицевая панель прибора снабжается цветовым  индикатором, который сообщает текущий режим работы. Также для пользователя представлено два краника, который в свою очередь имеет определенный цвет. Есть лицевая панель где можно выбрать определенную температуру охлаждения, нагрева, газирование и фильтрация.</t>
-  </si>
-  <si>
-    <t>Мощность охлождения 100Вт, мощность нагрева 550 Вт, энергопотребляемость 2 кВт*ч/сутки.</t>
-  </si>
-  <si>
-    <t>Так как прибор выполнен из качественного сырья и имеет обязательные и необязательные функции имеет увеличеную стоимость, поэтому потребность в данном приборе несколько снижена, но имеет много преимуществ.</t>
-  </si>
-  <si>
-    <t>Данный прибор имеет увеличиную мощность и дополнительную габаритность за счет холодильной камеры. Также прибор требует дополнительный расход на фильтрационный картридж.</t>
-  </si>
-  <si>
-    <t>Прибор имеет отдельный отдел для озонирывания посуды, также есть антибактериальное покрытие.</t>
-  </si>
-  <si>
-    <t>Cooler PRO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
+  <si>
+    <t>Полнота</t>
+  </si>
+  <si>
+    <t>Понятность</t>
+  </si>
+  <si>
+    <t>Правильность</t>
+  </si>
+  <si>
+    <t>Тестированность</t>
+  </si>
+  <si>
+    <t>Измеримость</t>
+  </si>
+  <si>
+    <t>Непротиворечивость</t>
+  </si>
+  <si>
+    <t>1. Нужен малогаборитный кулер с красивым дизайном. Вода должна быть постоянно холодной</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2. Нужен переностной кулер с компактным размером. При нажатии на кнопку, должен быть стакан с водой.</t>
+  </si>
+  <si>
+    <t>3.Нужен кулер который мог выдать воду минирализированую. Имел дистанционное управление.</t>
+  </si>
+  <si>
+    <t>4. Нужен кулер который дает сладкую газированую углекислым газом воду с температурой 80 градусов по Цельсию. Кулер потребляет электроэнергию 1 кВт*ч/день</t>
+  </si>
+  <si>
+    <t>5. Нужен кулер который имеет пропелер для передвижения по воздуху. Грузоподьемность кулера с емкостью 4 литра состовляет 6 кг, имеет аккамулятор с подзарядкой 220 В.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.Нужен кулер у которого карказ выполнен из дерева, имел глянцевую поверхность. Выдавал воду с клубничным сиропом, температура выданой жидкости состовляет 80 градусов за Цельсием. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +127,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -175,20 +167,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -215,6 +198,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -222,42 +214,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -540,131 +517,202 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="22"/>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:11" ht="312.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+        <v>11</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>7</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="122.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>8</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>7</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="4"/>
@@ -672,15 +720,11 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -688,15 +732,11 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -704,10 +744,8 @@
       <c r="K10" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
   </mergeCells>

</xml_diff>

<commit_message>
Story 6:Edit serial fot Testing Cooler
</commit_message>
<xml_diff>
--- a/Homework_1/Cooler_Requirements_Vlad_Dmytrenko.xlsx
+++ b/Homework_1/Cooler_Requirements_Vlad_Dmytrenko.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Полнота</t>
   </si>
@@ -42,12 +42,6 @@
     <t>1. Нужен малогаборитный кулер с красивым дизайном. Вода должна быть постоянно холодной</t>
   </si>
   <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>2. Нужен переностной кулер с компактным размером. При нажатии на кнопку, должен быть стакан с водой.</t>
   </si>
   <si>
@@ -61,13 +55,85 @@
   </si>
   <si>
     <t xml:space="preserve">6.Нужен кулер у которого карказ выполнен из дерева, имел глянцевую поверхность. Выдавал воду с клубничным сиропом, температура выданой жидкости состовляет 80 градусов за Цельсием. </t>
+  </si>
+  <si>
+    <t>7. Нужен кулер прямоугольной формы, выполнен из стекла, выдает квас 0,33 литра за 5 секунд.</t>
+  </si>
+  <si>
+    <t>не имеет всю инфлормацию для проектирывания</t>
+  </si>
+  <si>
+    <t>кулер-прямоугольной формы, выполнен из стекла, выдает квас</t>
+  </si>
+  <si>
+    <t>кулер выдает квас</t>
+  </si>
+  <si>
+    <t>выдает квас 0,33 литра за 5 секунд можно протестирывать</t>
+  </si>
+  <si>
+    <t>нельзя доказать соответсвие системы предьявленому требыванию</t>
+  </si>
+  <si>
+    <t>требывание не протеворечит другим требываниям</t>
+  </si>
+  <si>
+    <t>8.Кулер овальной формы, имеет синий цвет, матовый, выдает кисель. Энергоефективность кулера 2 кВт*ч/сутки при мощности ТЕНа 550 Вт. Температура воды при нагреве должна быть строго 95 градусов за Цельсием.</t>
+  </si>
+  <si>
+    <t>кулер овальной формы, синий цвет, матовый.</t>
+  </si>
+  <si>
+    <t>кулер выдает кисель</t>
+  </si>
+  <si>
+    <t>Энергоэфективность 2кВт*ч/сутки при мощности ТЕНа 550 Вт.</t>
+  </si>
+  <si>
+    <t>Температура воды при нагреве должна быть строго 95 градусов за Цельсием.</t>
+  </si>
+  <si>
+    <t>Требывание имеет двусмысленный характер</t>
+  </si>
+  <si>
+    <t>нет точного описания того, что должно быть разработано</t>
+  </si>
+  <si>
+    <t>не возможно протыстирывать</t>
+  </si>
+  <si>
+    <t>Кулер выдает воду</t>
+  </si>
+  <si>
+    <t>кулер  дает сладкую газированую углекислым газом воду, кулер потребляет электроэнергию 1 кВт*ч/день</t>
+  </si>
+  <si>
+    <t>Кулер выдает сладкую газырованую воду</t>
+  </si>
+  <si>
+    <t>Кулер потребляет электроэнергию 1 кВт*ч/день</t>
+  </si>
+  <si>
+    <t>кулер выдает воду с температурой 80 градусов по Цельсию</t>
+  </si>
+  <si>
+    <t>Грузоподьемность кулера с емкостью 4 литра состовляет 6 кг</t>
+  </si>
+  <si>
+    <t>кулер выполнен из дерева, имеет глянцевую поверхность, выдает воду с клубничным сиропом</t>
+  </si>
+  <si>
+    <t>кулер выдает воду с сиропом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">температура выданой жидкости состовляет 80 градусов за Цельсием. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,20 +181,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -171,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -207,34 +259,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -517,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,23 +573,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -557,46 +597,46 @@
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>7</v>
+      <c r="B2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="19" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -605,48 +645,48 @@
     </row>
     <row r="4" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>8</v>
+      <c r="B4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -655,25 +695,25 @@
     </row>
     <row r="6" spans="1:11" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -682,25 +722,25 @@
     </row>
     <row r="7" spans="1:11" ht="162" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>7</v>
+      <c r="C7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -708,24 +748,54 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="11"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="4"/>
+      <c r="A8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="3"/>
+    <row r="9" spans="1:11" ht="177" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -735,8 +805,8 @@
       <c r="A10" s="10"/>
       <c r="B10" s="12"/>
       <c r="C10" s="11"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -744,10 +814,8 @@
       <c r="K10" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>